<commit_message>
Final few changes, small additions to analysis of data.
</commit_message>
<xml_diff>
--- a/data/raw/gorilla/ppt_groups.xlsx
+++ b/data/raw/gorilla/ppt_groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e1e47eb9dffef9f/Documents/All Documents/University/Sheffield/Dissertation/caffeine_and_ADHD_dissertation/data/raw/gorilla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{09F78766-A1B3-43D5-8A6C-C7E056EBCCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2BC1D21-567A-4891-A771-410B916D07EF}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{09F78766-A1B3-43D5-8A6C-C7E056EBCCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EC74373-E764-48F1-873C-84A48C25EBAC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B937B225-D68A-6E46-BA6F-256820BFD70D}"/>
   </bookViews>
@@ -37,12 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="9">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -62,6 +56,12 @@
   </si>
   <si>
     <t>age</t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t>Caffeine</t>
   </si>
 </sst>
 </file>
@@ -423,27 +423,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694B2300-A81F-F74B-91AA-9F73C03B86CC}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -454,10 +454,10 @@
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>26</v>
@@ -471,10 +471,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>57</v>
@@ -488,10 +488,10 @@
         <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>40</v>
@@ -505,10 +505,10 @@
         <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>42</v>
@@ -522,10 +522,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>46</v>
@@ -539,10 +539,10 @@
         <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>61</v>
@@ -556,10 +556,10 @@
         <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>46</v>
@@ -573,10 +573,10 @@
         <v>116</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>58</v>
@@ -590,10 +590,10 @@
         <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>62</v>
@@ -607,10 +607,10 @@
         <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>22</v>
@@ -624,10 +624,10 @@
         <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>23</v>
@@ -641,10 +641,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>22</v>
@@ -658,10 +658,10 @@
         <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>44</v>
@@ -675,10 +675,10 @@
         <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>21</v>
@@ -692,10 +692,10 @@
         <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>30</v>
@@ -709,10 +709,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>33</v>
@@ -726,10 +726,10 @@
         <v>125</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>21</v>
@@ -743,10 +743,10 @@
         <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>24</v>
@@ -760,10 +760,10 @@
         <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>35</v>
@@ -777,10 +777,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>24</v>
@@ -794,10 +794,10 @@
         <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>22</v>
@@ -811,10 +811,10 @@
         <v>96</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>29</v>
@@ -828,10 +828,10 @@
         <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>50</v>
@@ -845,10 +845,10 @@
         <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>29</v>
@@ -862,10 +862,10 @@
         <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>20</v>
@@ -879,10 +879,10 @@
         <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>22</v>
@@ -896,10 +896,10 @@
         <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>23</v>
@@ -913,10 +913,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>32</v>
@@ -930,10 +930,10 @@
         <v>113</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>22</v>
@@ -947,10 +947,10 @@
         <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>23</v>
@@ -964,10 +964,10 @@
         <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>32</v>
@@ -981,10 +981,10 @@
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>21</v>
@@ -998,10 +998,10 @@
         <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>22</v>
@@ -1015,10 +1015,10 @@
         <v>99</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>31</v>
@@ -1032,10 +1032,10 @@
         <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>22</v>
@@ -1049,10 +1049,10 @@
         <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>23</v>
@@ -1066,10 +1066,10 @@
         <v>92</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>25</v>
@@ -1083,10 +1083,10 @@
         <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>32</v>
@@ -1100,10 +1100,10 @@
         <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>31</v>
@@ -1117,10 +1117,10 @@
         <v>124</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>33</v>
@@ -1134,10 +1134,10 @@
         <v>97</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>18</v>
@@ -1151,10 +1151,10 @@
         <v>98</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>22</v>
@@ -1168,10 +1168,10 @@
         <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>22</v>
@@ -1185,10 +1185,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>28</v>
@@ -1202,10 +1202,10 @@
         <v>129</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46">
         <v>22</v>
@@ -1219,10 +1219,10 @@
         <v>5</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>42</v>
@@ -1236,10 +1236,10 @@
         <v>80</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>57</v>
@@ -1253,10 +1253,10 @@
         <v>74</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>25</v>
@@ -1270,10 +1270,10 @@
         <v>39</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>32</v>
@@ -1287,10 +1287,10 @@
         <v>112</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>44</v>
@@ -1304,10 +1304,10 @@
         <v>101</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>26</v>
@@ -1321,10 +1321,10 @@
         <v>79</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>29</v>
@@ -1338,10 +1338,10 @@
         <v>102</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E54">
         <v>23</v>
@@ -1355,10 +1355,10 @@
         <v>128</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E55">
         <v>32</v>
@@ -1372,10 +1372,10 @@
         <v>72</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>22</v>
@@ -1389,10 +1389,10 @@
         <v>49</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>24</v>
@@ -1406,10 +1406,10 @@
         <v>87</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E58">
         <v>48</v>
@@ -1423,10 +1423,10 @@
         <v>33</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>19</v>
@@ -1440,10 +1440,10 @@
         <v>91</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>22</v>
@@ -1457,10 +1457,10 @@
         <v>44</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>55</v>
@@ -1474,10 +1474,10 @@
         <v>115</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>32</v>
@@ -1491,10 +1491,10 @@
         <v>127</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>34</v>
@@ -1508,10 +1508,10 @@
         <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>24</v>

</xml_diff>